<commit_message>
Updated MoM for meeting on 25th Jan 2018
</commit_message>
<xml_diff>
--- a/4. Project Monitoring & Control/Communication/Minutes of Meetings/ABRS_MinutesOfMeetings.xlsx
+++ b/4. Project Monitoring & Control/Communication/Minutes of Meetings/ABRS_MinutesOfMeetings.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AORS\4. Project Monitoring &amp; Control\Communication\Minutes of Meetings\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ABRS\4. Project Monitoring &amp; Control\Communication\Minutes of Meetings\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -297,7 +297,7 @@
     <t>Shared to Durva via Whatsapp</t>
   </si>
   <si>
-    <t>Suggested Sunday over phone call.</t>
+    <t xml:space="preserve">Every Sunday 10:30 am </t>
   </si>
 </sst>
 </file>
@@ -1313,13 +1313,46 @@
     <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1350,39 +1383,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="15" fontId="15" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1744,13 +1744,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -3903,35 +3903,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="126" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="116"/>
-      <c r="C1" s="116"/>
-      <c r="D1" s="116"/>
-      <c r="E1" s="116"/>
-      <c r="F1" s="116"/>
-      <c r="G1" s="117"/>
+      <c r="B1" s="127"/>
+      <c r="C1" s="127"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="127"/>
+      <c r="F1" s="127"/>
+      <c r="G1" s="128"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="118" t="s">
+      <c r="A2" s="129" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="119" t="s">
+      <c r="B2" s="130" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="119"/>
-      <c r="D2" s="119" t="s">
+      <c r="C2" s="130"/>
+      <c r="D2" s="130" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="119"/>
-      <c r="F2" s="119" t="s">
+      <c r="E2" s="130"/>
+      <c r="F2" s="130" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="120"/>
+      <c r="G2" s="131"/>
     </row>
     <row r="3" spans="1:12" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="118"/>
+      <c r="A3" s="129"/>
       <c r="B3" s="37" t="s">
         <v>16</v>
       </c>
@@ -3950,10 +3950,10 @@
       <c r="G3" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="112"/>
-      <c r="J3" s="112"/>
-      <c r="K3" s="112"/>
-      <c r="L3" s="112"/>
+      <c r="I3" s="125"/>
+      <c r="J3" s="125"/>
+      <c r="K3" s="125"/>
+      <c r="L3" s="125"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="31" t="s">
@@ -3977,10 +3977,10 @@
       <c r="G4" s="58">
         <v>40190</v>
       </c>
-      <c r="I4" s="112"/>
-      <c r="J4" s="112"/>
-      <c r="K4" s="112"/>
-      <c r="L4" s="112"/>
+      <c r="I4" s="125"/>
+      <c r="J4" s="125"/>
+      <c r="K4" s="125"/>
+      <c r="L4" s="125"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="54" t="s">
@@ -4102,96 +4102,96 @@
       <c r="A11" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="121" t="s">
+      <c r="B11" s="132" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="121"/>
-      <c r="D11" s="121"/>
-      <c r="E11" s="121"/>
-      <c r="F11" s="121"/>
-      <c r="G11" s="122"/>
+      <c r="C11" s="132"/>
+      <c r="D11" s="132"/>
+      <c r="E11" s="132"/>
+      <c r="F11" s="132"/>
+      <c r="G11" s="133"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="123" t="s">
+      <c r="B12" s="134" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="123"/>
-      <c r="D12" s="123"/>
-      <c r="E12" s="123"/>
-      <c r="F12" s="123"/>
-      <c r="G12" s="124"/>
-      <c r="I12" s="112"/>
-      <c r="J12" s="112"/>
-      <c r="K12" s="112"/>
-      <c r="L12" s="112"/>
+      <c r="C12" s="134"/>
+      <c r="D12" s="134"/>
+      <c r="E12" s="134"/>
+      <c r="F12" s="134"/>
+      <c r="G12" s="135"/>
+      <c r="I12" s="125"/>
+      <c r="J12" s="125"/>
+      <c r="K12" s="125"/>
+      <c r="L12" s="125"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="123" t="s">
+      <c r="B13" s="134" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="123"/>
-      <c r="D13" s="123"/>
-      <c r="E13" s="123"/>
-      <c r="F13" s="123"/>
-      <c r="G13" s="124"/>
+      <c r="C13" s="134"/>
+      <c r="D13" s="134"/>
+      <c r="E13" s="134"/>
+      <c r="F13" s="134"/>
+      <c r="G13" s="135"/>
     </row>
     <row r="14" spans="1:12" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A14" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="123" t="s">
+      <c r="B14" s="134" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="123"/>
-      <c r="D14" s="123"/>
-      <c r="E14" s="123"/>
-      <c r="F14" s="123"/>
-      <c r="G14" s="124"/>
+      <c r="C14" s="134"/>
+      <c r="D14" s="134"/>
+      <c r="E14" s="134"/>
+      <c r="F14" s="134"/>
+      <c r="G14" s="135"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="55">
         <v>2</v>
       </c>
-      <c r="B15" s="113" t="s">
+      <c r="B15" s="118" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="113"/>
-      <c r="D15" s="113"/>
-      <c r="E15" s="113"/>
-      <c r="F15" s="113"/>
-      <c r="G15" s="114"/>
+      <c r="C15" s="118"/>
+      <c r="D15" s="118"/>
+      <c r="E15" s="118"/>
+      <c r="F15" s="118"/>
+      <c r="G15" s="119"/>
     </row>
     <row r="16" spans="1:12" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A16" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="113" t="s">
+      <c r="B16" s="118" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="113"/>
-      <c r="D16" s="113"/>
-      <c r="E16" s="113"/>
-      <c r="F16" s="113"/>
-      <c r="G16" s="114"/>
+      <c r="C16" s="118"/>
+      <c r="D16" s="118"/>
+      <c r="E16" s="118"/>
+      <c r="F16" s="118"/>
+      <c r="G16" s="119"/>
     </row>
     <row r="17" spans="1:9" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="130" t="s">
+      <c r="B17" s="122" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="131"/>
-      <c r="D17" s="131"/>
-      <c r="E17" s="131"/>
-      <c r="F17" s="131"/>
-      <c r="G17" s="132"/>
+      <c r="C17" s="123"/>
+      <c r="D17" s="123"/>
+      <c r="E17" s="123"/>
+      <c r="F17" s="123"/>
+      <c r="G17" s="124"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="38"/>
@@ -4206,82 +4206,82 @@
     </row>
     <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="125" t="s">
+      <c r="A20" s="112" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="125"/>
-      <c r="C20" s="125"/>
-      <c r="D20" s="125"/>
-      <c r="E20" s="125"/>
+      <c r="B20" s="112"/>
+      <c r="C20" s="112"/>
+      <c r="D20" s="112"/>
+      <c r="E20" s="112"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="126" t="s">
+      <c r="A21" s="120" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="126"/>
-      <c r="C21" s="127" t="s">
+      <c r="B21" s="120"/>
+      <c r="C21" s="121" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="127"/>
-      <c r="E21" s="127"/>
+      <c r="D21" s="121"/>
+      <c r="E21" s="121"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="128"/>
-      <c r="B22" s="128"/>
-      <c r="C22" s="129"/>
-      <c r="D22" s="129"/>
-      <c r="E22" s="129"/>
+      <c r="A22" s="117"/>
+      <c r="B22" s="117"/>
+      <c r="C22" s="114"/>
+      <c r="D22" s="114"/>
+      <c r="E22" s="114"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="128"/>
-      <c r="B23" s="128"/>
-      <c r="C23" s="129"/>
-      <c r="D23" s="129"/>
-      <c r="E23" s="129"/>
+      <c r="A23" s="117"/>
+      <c r="B23" s="117"/>
+      <c r="C23" s="114"/>
+      <c r="D23" s="114"/>
+      <c r="E23" s="114"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="128"/>
-      <c r="B24" s="128"/>
-      <c r="C24" s="129"/>
-      <c r="D24" s="129"/>
-      <c r="E24" s="129"/>
+      <c r="A24" s="117"/>
+      <c r="B24" s="117"/>
+      <c r="C24" s="114"/>
+      <c r="D24" s="114"/>
+      <c r="E24" s="114"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="128"/>
-      <c r="B25" s="128"/>
-      <c r="C25" s="129"/>
-      <c r="D25" s="129"/>
-      <c r="E25" s="129"/>
+      <c r="A25" s="117"/>
+      <c r="B25" s="117"/>
+      <c r="C25" s="114"/>
+      <c r="D25" s="114"/>
+      <c r="E25" s="114"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="133"/>
-      <c r="B26" s="133"/>
-      <c r="C26" s="129"/>
-      <c r="D26" s="129"/>
-      <c r="E26" s="129"/>
+      <c r="A26" s="113"/>
+      <c r="B26" s="113"/>
+      <c r="C26" s="114"/>
+      <c r="D26" s="114"/>
+      <c r="E26" s="114"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="133"/>
-      <c r="B27" s="133"/>
-      <c r="C27" s="129"/>
-      <c r="D27" s="129"/>
-      <c r="E27" s="129"/>
+      <c r="A27" s="113"/>
+      <c r="B27" s="113"/>
+      <c r="C27" s="114"/>
+      <c r="D27" s="114"/>
+      <c r="E27" s="114"/>
     </row>
     <row r="28" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="134"/>
-      <c r="B28" s="134"/>
-      <c r="C28" s="135"/>
-      <c r="D28" s="135"/>
-      <c r="E28" s="135"/>
+      <c r="A28" s="115"/>
+      <c r="B28" s="115"/>
+      <c r="C28" s="116"/>
+      <c r="D28" s="116"/>
+      <c r="E28" s="116"/>
     </row>
     <row r="29" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="125" t="s">
+      <c r="A30" s="112" t="s">
         <v>22</v>
       </c>
-      <c r="B30" s="125"/>
-      <c r="C30" s="125"/>
-      <c r="D30" s="125"/>
+      <c r="B30" s="112"/>
+      <c r="C30" s="112"/>
+      <c r="D30" s="112"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="36" t="s">
@@ -4342,26 +4342,6 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="32">
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="B17:G17"/>
     <mergeCell ref="I3:L4"/>
     <mergeCell ref="B15:G15"/>
     <mergeCell ref="A1:G1"/>
@@ -4374,6 +4354,26 @@
     <mergeCell ref="I12:L12"/>
     <mergeCell ref="B13:G13"/>
     <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C28:E28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4430,7 +4430,7 @@
       </c>
       <c r="B4" s="65">
         <f>COUNTIF(MOM!J:J,A4)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
@@ -4448,7 +4448,7 @@
       </c>
       <c r="B6" s="66">
         <f>COUNTIF(MOM!J:J,A6)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
@@ -4487,10 +4487,10 @@
   </sheetPr>
   <dimension ref="A1:CH65523"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G17" sqref="G17"/>
-      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.35"/>
@@ -4734,9 +4734,11 @@
       <c r="H3" s="83">
         <v>43126</v>
       </c>
-      <c r="I3" s="83"/>
+      <c r="I3" s="83">
+        <v>43130</v>
+      </c>
       <c r="J3" s="84" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K3" s="85"/>
       <c r="L3" s="14"/>
@@ -4830,9 +4832,11 @@
       <c r="H4" s="80">
         <v>43126</v>
       </c>
-      <c r="I4" s="80"/>
+      <c r="I4" s="80">
+        <v>43130</v>
+      </c>
       <c r="J4" s="81" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K4" s="86" t="s">
         <v>71</v>

</xml_diff>

<commit_message>
Updated MoM for meeting on 11-02-2018
</commit_message>
<xml_diff>
--- a/4. Project Monitoring & Control/Communication/Minutes of Meetings/ABRS_MinutesOfMeetings.xlsx
+++ b/4. Project Monitoring & Control/Communication/Minutes of Meetings/ABRS_MinutesOfMeetings.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="80">
   <si>
     <t>Attendees</t>
   </si>
@@ -298,6 +298,33 @@
   </si>
   <si>
     <t xml:space="preserve">Every Sunday 10:30 am </t>
+  </si>
+  <si>
+    <t>Weekly Status Report
+GitHub initialization</t>
+  </si>
+  <si>
+    <t>120 Minutes</t>
+  </si>
+  <si>
+    <t>Devaj Parikh, Durva Shah, Sadhika Sajeev</t>
+  </si>
+  <si>
+    <t>Work-plan for next week.
+Git installation
+Repository cloning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To help in setup of GitBash repository and cloning installation details  </t>
+  </si>
+  <si>
+    <t>Sadhika Sajeev</t>
+  </si>
+  <si>
+    <t>Complete all tutorials assigned in Kick-off meeting</t>
+  </si>
+  <si>
+    <t>Help other team members in installing coding related softwares.</t>
   </si>
 </sst>
 </file>
@@ -1000,7 +1027,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="156">
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1416,6 +1443,33 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4490,7 +4544,7 @@
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G17" sqref="G17"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.35"/>
@@ -5118,27 +5172,27 @@
       <c r="CH6" s="14"/>
     </row>
     <row r="7" spans="1:86" ht="53.4" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="140"/>
-      <c r="B7" s="143"/>
-      <c r="C7" s="143"/>
-      <c r="D7" s="143"/>
-      <c r="E7" s="146"/>
-      <c r="F7" s="87" t="s">
+      <c r="A7" s="152"/>
+      <c r="B7" s="153"/>
+      <c r="C7" s="153"/>
+      <c r="D7" s="153"/>
+      <c r="E7" s="154"/>
+      <c r="F7" s="147" t="s">
         <v>66</v>
       </c>
-      <c r="G7" s="87" t="s">
+      <c r="G7" s="147" t="s">
         <v>67</v>
       </c>
-      <c r="H7" s="88">
+      <c r="H7" s="148">
         <v>43126</v>
       </c>
-      <c r="I7" s="88">
+      <c r="I7" s="148">
         <v>43126</v>
       </c>
-      <c r="J7" s="89" t="s">
+      <c r="J7" s="149" t="s">
         <v>44</v>
       </c>
-      <c r="K7" s="90" t="s">
+      <c r="K7" s="150" t="s">
         <v>68</v>
       </c>
       <c r="L7" s="14"/>
@@ -5217,14 +5271,34 @@
       <c r="CG7" s="14"/>
       <c r="CH7" s="14"/>
     </row>
-    <row r="8" spans="1:86" x14ac:dyDescent="0.35">
-      <c r="A8" s="77"/>
-      <c r="B8" s="77"/>
-      <c r="C8" s="77"/>
-      <c r="D8" s="77"/>
-      <c r="E8" s="78"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
+    <row r="8" spans="1:86" ht="39.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="138">
+        <v>43142</v>
+      </c>
+      <c r="B8" s="141" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="141" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" s="141" t="s">
+        <v>74</v>
+      </c>
+      <c r="E8" s="144" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" s="82" t="s">
+        <v>76</v>
+      </c>
+      <c r="G8" s="82" t="s">
+        <v>77</v>
+      </c>
+      <c r="H8" s="83">
+        <v>43144</v>
+      </c>
+      <c r="I8" s="83"/>
+      <c r="J8" s="84"/>
+      <c r="K8" s="85"/>
       <c r="L8" s="14"/>
       <c r="M8" s="14"/>
       <c r="N8" s="14"/>
@@ -5301,14 +5375,24 @@
       <c r="CG8" s="14"/>
       <c r="CH8" s="14"/>
     </row>
-    <row r="9" spans="1:86" x14ac:dyDescent="0.35">
-      <c r="A9" s="77"/>
-      <c r="B9" s="77"/>
-      <c r="C9" s="77"/>
-      <c r="D9" s="77"/>
-      <c r="E9" s="78"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
+    <row r="9" spans="1:86" ht="52.8" x14ac:dyDescent="0.35">
+      <c r="A9" s="139"/>
+      <c r="B9" s="142"/>
+      <c r="C9" s="142"/>
+      <c r="D9" s="142"/>
+      <c r="E9" s="145"/>
+      <c r="F9" s="79" t="s">
+        <v>78</v>
+      </c>
+      <c r="G9" s="79" t="s">
+        <v>67</v>
+      </c>
+      <c r="H9" s="80">
+        <v>43148</v>
+      </c>
+      <c r="I9" s="80"/>
+      <c r="J9" s="81"/>
+      <c r="K9" s="86"/>
       <c r="L9" s="14"/>
       <c r="M9" s="14"/>
       <c r="N9" s="14"/>
@@ -5385,14 +5469,22 @@
       <c r="CG9" s="14"/>
       <c r="CH9" s="14"/>
     </row>
-    <row r="10" spans="1:86" x14ac:dyDescent="0.35">
-      <c r="A10" s="77"/>
-      <c r="B10" s="77"/>
-      <c r="C10" s="77"/>
-      <c r="D10" s="77"/>
-      <c r="E10" s="78"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
+    <row r="10" spans="1:86" ht="53.4" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="140"/>
+      <c r="B10" s="143"/>
+      <c r="C10" s="143"/>
+      <c r="D10" s="143"/>
+      <c r="E10" s="146"/>
+      <c r="F10" s="155" t="s">
+        <v>79</v>
+      </c>
+      <c r="G10" s="87" t="s">
+        <v>67</v>
+      </c>
+      <c r="H10" s="88"/>
+      <c r="I10" s="88"/>
+      <c r="J10" s="89"/>
+      <c r="K10" s="90"/>
       <c r="L10" s="14"/>
       <c r="M10" s="14"/>
       <c r="N10" s="14"/>
@@ -5469,15 +5561,14 @@
       <c r="CG10" s="14"/>
       <c r="CH10" s="14"/>
     </row>
-    <row r="11" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:86" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="77"/>
       <c r="B11" s="77"/>
       <c r="C11" s="77"/>
       <c r="D11" s="77"/>
-      <c r="E11" s="78"/>
+      <c r="E11" s="151"/>
       <c r="H11" s="17"/>
       <c r="I11" s="17"/>
-      <c r="J11" s="67"/>
       <c r="L11" s="14"/>
       <c r="M11" s="14"/>
       <c r="N11" s="14"/>
@@ -5554,15 +5645,14 @@
       <c r="CG11" s="14"/>
       <c r="CH11" s="14"/>
     </row>
-    <row r="12" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:86" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="77"/>
       <c r="B12" s="77"/>
       <c r="C12" s="77"/>
       <c r="D12" s="77"/>
-      <c r="E12" s="78"/>
+      <c r="E12" s="151"/>
       <c r="H12" s="17"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="67"/>
+      <c r="I12" s="17"/>
       <c r="L12" s="14"/>
       <c r="M12" s="14"/>
       <c r="N12" s="14"/>
@@ -57981,12 +58071,17 @@
     </row>
   </sheetData>
   <autoFilter ref="A2:K74" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
-  <mergeCells count="5">
+  <mergeCells count="10">
     <mergeCell ref="A3:A7"/>
     <mergeCell ref="B3:B7"/>
     <mergeCell ref="C3:C7"/>
     <mergeCell ref="D3:D7"/>
     <mergeCell ref="E3:E7"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="1">

</xml_diff>